<commit_message>
Try halving pepper instead of quartering first
</commit_message>
<xml_diff>
--- a/temperatures.xlsx
+++ b/temperatures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ana/Documents/recipes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBDC519-2274-E64D-B0F5-4D9C4DA17B6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58FFDC6C-CF61-E143-9DA5-70E6A434F8C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sizzle &amp; Sear" sheetId="3" r:id="rId1"/>
@@ -1738,7 +1738,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B20" sqref="B20:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="65.6640625" defaultRowHeight="19" x14ac:dyDescent="0.25"/>

</xml_diff>